<commit_message>
0000988: Ajout des notions d'état civil sur RQ_L2_DOC
</commit_message>
<xml_diff>
--- a/GestVAE/DOCS/Réponse1405.xlsx
+++ b/GestVAE/DOCS/Réponse1405.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\2pConsultants\EHESP\APP\gestVAE\GestVAE\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF9555-D9C0-4AD9-A3B8-6978163EAC5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132C8515-D278-486B-B2ED-02E7E4DF18AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10185" xr2:uid="{AB284223-390E-4CD9-B888-2D9470CF466D}"/>
   </bookViews>
@@ -183,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,19 +191,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,289 +542,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58902F4-F4DC-437B-9B8C-933CA4412016}">
-  <sheetPr codeName="Feuil1" filterMode="1"/>
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>13</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>15</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E20" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="F20" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20" xr:uid="{C1D513CE-6377-49A8-8FBA-9C8071392A93}">
-    <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="OK"/>
-        <filter val="OUI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E20" xr:uid="{C1D513CE-6377-49A8-8FBA-9C8071392A93}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>